<commit_message>
Added Jefferson and changed the date.
</commit_message>
<xml_diff>
--- a/File.xlsx
+++ b/File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d42433aad8bf578/Python GIT/Auto-mail/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\source\repos\Mail-Sende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{088C7B64-4633-4931-A0FB-F63B63033927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0B5B6DF0-2FB7-4F87-B331-F09F1C6D6E82}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25856EA-B98A-40C0-BF7D-2E3EFE22CE02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{845DE247-813B-4D28-8501-4FD3E15F0A98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{845DE247-813B-4D28-8501-4FD3E15F0A98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Nome</t>
   </si>
@@ -61,6 +52,12 @@
   </si>
   <si>
     <t>5 hours</t>
+  </si>
+  <si>
+    <t>Jefferson André</t>
+  </si>
+  <si>
+    <t>jefferson.andre96@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -427,20 +424,20 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -468,30 +465,45 @@
         <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>80832</v>
+        <v>44308</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44308</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{FFFAE6E8-7F75-4F90-B0FF-70CC136354D9}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{9915885A-B840-46EA-B57C-4FD2881B546A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>